<commit_message>
Asset, Assetliste & Zeiterfassung
</commit_message>
<xml_diff>
--- a/_WIP/Michelle/Michelle-Zeiterfassung.xlsx
+++ b/_WIP/Michelle/Michelle-Zeiterfassung.xlsx
@@ -1111,7 +1111,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1121,8 +1121,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H184"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="G91" sqref="G91"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="D106" sqref="D106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3021,12 +3021,14 @@
       <c r="A106" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="B106" s="13"/>
+      <c r="B106" s="13">
+        <v>0.36458333333333331</v>
+      </c>
       <c r="C106" s="13"/>
       <c r="D106" s="23"/>
       <c r="E106" s="9">
         <f>(B106-C106)*-24-D106</f>
-        <v>0</v>
+        <v>-8.75</v>
       </c>
       <c r="F106" s="12"/>
       <c r="G106" s="12"/>
@@ -3131,7 +3133,7 @@
       </c>
       <c r="E113" s="27">
         <f>SUM(E106:E112)</f>
-        <v>0</v>
+        <v>-8.75</v>
       </c>
       <c r="F113" s="2"/>
       <c r="G113" s="2"/>
@@ -3146,7 +3148,7 @@
       </c>
       <c r="E114" s="22">
         <f>SUM(E13+E23+E33+E43+E53+E63+E73+E83+E93+E103+E113)</f>
-        <v>137.5</v>
+        <v>128.75</v>
       </c>
       <c r="F114" s="3"/>
       <c r="G114" s="3"/>
@@ -3307,7 +3309,7 @@
       </c>
       <c r="E124" s="22">
         <f>SUM(E13+E23+E33+E43+E53+E63+E73+E83+E93+E103+E113+E123)</f>
-        <v>137.5</v>
+        <v>128.75</v>
       </c>
       <c r="F124" s="3"/>
       <c r="G124" s="3"/>
@@ -3468,7 +3470,7 @@
       </c>
       <c r="E134" s="22">
         <f>SUM(E13+E23+E33+E43+E53+E63+E73+E83+E93+E103+E113+E123+E133)</f>
-        <v>137.5</v>
+        <v>128.75</v>
       </c>
       <c r="F134" s="3"/>
       <c r="G134" s="3"/>
@@ -3629,7 +3631,7 @@
       </c>
       <c r="E144" s="22">
         <f>SUM(E13+E23+E33+E43+E53+E63+E73+E83+E93+E103+E113+E123+E133+E143)</f>
-        <v>137.5</v>
+        <v>128.75</v>
       </c>
       <c r="F144" s="3"/>
       <c r="G144" s="3"/>
@@ -3790,7 +3792,7 @@
       </c>
       <c r="E154" s="22">
         <f>SUM(E13+E23+E33+E43+E53+E63+E73+E83+E93+E103+E113+E123+E133+E143+E153)</f>
-        <v>137.5</v>
+        <v>128.75</v>
       </c>
       <c r="F154" s="3"/>
       <c r="G154" s="3"/>
@@ -3950,7 +3952,7 @@
       </c>
       <c r="E164" s="22">
         <f>SUM(E13+E23+E33+E43+E53+E63+E73+E83+E93+E103+E113+E123+E133+E143+E153+E163)</f>
-        <v>137.5</v>
+        <v>128.75</v>
       </c>
       <c r="F164" s="3"/>
       <c r="G164" s="3"/>
@@ -4111,7 +4113,7 @@
       </c>
       <c r="E174" s="22">
         <f>SUM(E13+E23+E33+E43+E53+E63+E73+E83+E93+E103+E113+E123+E133+E143+E153+E163+E173)</f>
-        <v>137.5</v>
+        <v>128.75</v>
       </c>
       <c r="F174" s="3"/>
       <c r="G174" s="3"/>
@@ -4272,7 +4274,7 @@
       </c>
       <c r="E184" s="27">
         <f>SUM(E13+E23+E33+E43+E53+E63+E73+E83+E93+E103+E113+E123+E133+E143+E153+E163+E173+E183)</f>
-        <v>137.5</v>
+        <v>128.75</v>
       </c>
       <c r="F184" s="2"/>
       <c r="G184" s="2"/>

</xml_diff>

<commit_message>
Revert "Revert "Level überarbeitet""
This reverts commit a4f2a1a67a5e903111ff70d890d5e77878408fbe.
</commit_message>
<xml_diff>
--- a/_WIP/Michelle/Michelle-Zeiterfassung.xlsx
+++ b/_WIP/Michelle/Michelle-Zeiterfassung.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="169">
   <si>
     <t>Zeiterfassung</t>
   </si>
@@ -523,6 +523,9 @@
   </si>
   <si>
     <t>Assets überarbeitet, 3D Vergrößerungsglas</t>
+  </si>
+  <si>
+    <t>Assetliste, 3D Rührstab, 3D Schemel</t>
   </si>
 </sst>
 </file>
@@ -1114,7 +1117,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1125,7 +1128,7 @@
   <dimension ref="A1:H184"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="F107" sqref="F107"/>
+      <selection activeCell="J107" sqref="J107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3061,7 +3064,9 @@
         <v>6.75</v>
       </c>
       <c r="F107" s="12"/>
-      <c r="G107" s="12"/>
+      <c r="G107" s="12" t="s">
+        <v>168</v>
+      </c>
       <c r="H107" s="12"/>
     </row>
     <row r="108" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>